<commit_message>
ready to test the impact of epochs
</commit_message>
<xml_diff>
--- a/error/new/pp_and_da/pp_and_da_myval.xlsx
+++ b/error/new/pp_and_da/pp_and_da_myval.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>Classe</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Class\Opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>pp + f + r</t>
+  </si>
+  <si>
+    <t>pp\class</t>
   </si>
 </sst>
 </file>
@@ -1351,45 +1360,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1462,7 +1432,6 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2063,71 +2032,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.0194</cdr:x>
-      <cdr:y>0.74429</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.98547</cdr:x>
-      <cdr:y>0.77106</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="Retângulo 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7C3081F-459F-439C-A04D-EFC6F4EF9DE6}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="216568" y="4872951"/>
-          <a:ext cx="10784529" cy="175266"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </cdr:style>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2391,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V71"/>
+  <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J35" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="L17" workbookViewId="0">
+      <selection activeCell="AO14" sqref="AO14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2404,7 +2308,7 @@
     <col min="18" max="18" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
@@ -2436,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="2">
         <v>0</v>
@@ -2494,8 +2398,32 @@
         <v>128</v>
       </c>
       <c r="V2" s="8"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="8">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="8">
+        <v>5</v>
+      </c>
+      <c r="AF2" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="2">
         <v>1</v>
@@ -2561,8 +2489,33 @@
         <v>#DIV/0!</v>
       </c>
       <c r="V3" s="8"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3">
+        <f t="array" ref="Z3:AF7">TRANSPOSE(N3:R9)</f>
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>0.97334443981674301</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>0.92669720949604328</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="2">
         <v>2</v>
@@ -2628,8 +2581,32 @@
         <v>#DIV/0!</v>
       </c>
       <c r="V4" s="8"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z4">
+        <v>0.93294460641399413</v>
+      </c>
+      <c r="AA4">
+        <v>0.3715118700541441</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>6.4556434818825489E-2</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="2">
         <v>3</v>
@@ -2695,8 +2672,32 @@
         <v>#DIV/0!</v>
       </c>
       <c r="V5" s="8"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>0.93044564764681381</v>
+      </c>
+      <c r="AC5">
+        <v>0.9433569346105789</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="2">
         <v>4</v>
@@ -2762,8 +2763,35 @@
         <v>#DIV/0!</v>
       </c>
       <c r="V6" s="8"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>0.93544356518117455</v>
+      </c>
+      <c r="AC6">
+        <v>0.87880049979175345</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="2">
         <v>5</v>
@@ -2829,8 +2857,32 @@
         <v>#DIV/0!</v>
       </c>
       <c r="V7" s="8"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>0.8567263640149938</v>
+      </c>
+      <c r="AC7">
+        <v>0.89004581424406493</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="2">
         <v>6</v>
@@ -2897,7 +2949,7 @@
       </c>
       <c r="V8" s="8"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="M9" s="8">
         <v>6</v>
       </c>
@@ -2935,7 +2987,7 @@
       </c>
       <c r="V9" s="8"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
@@ -2977,7 +3029,7 @@
       <c r="U10" s="11"/>
       <c r="V10" s="8"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="2">
         <v>0</v>
@@ -3044,7 +3096,7 @@
       </c>
       <c r="V11" s="8"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="2">
         <v>1</v>
@@ -3111,7 +3163,7 @@
       </c>
       <c r="V12" s="8"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="2">
         <v>2</v>
@@ -3178,7 +3230,7 @@
       </c>
       <c r="V13" s="8"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="2">
         <v>3</v>
@@ -3245,7 +3297,7 @@
       </c>
       <c r="V14" s="8"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="2">
         <v>4</v>
@@ -3286,7 +3338,7 @@
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
ready to move on to study the impact of the number of epochs
</commit_message>
<xml_diff>
--- a/error/new/pp_and_da/pp_and_da_myval.xlsx
+++ b/error/new/pp_and_da/pp_and_da_myval.xlsx
@@ -1360,6 +1360,45 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1432,6 +1471,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2032,6 +2072,71 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.01775</cdr:x>
+      <cdr:y>0.74197</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.9884</cdr:x>
+      <cdr:y>0.77107</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Retângulo 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0E80E5A-BDB8-4F55-8662-080AAC15DCC5}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="198120" y="4857750"/>
+          <a:ext cx="10835640" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2298,7 +2403,7 @@
   <dimension ref="A1:AF71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L17" workbookViewId="0">
-      <selection activeCell="AO14" sqref="AO14"/>
+      <selection activeCell="AF35" sqref="AF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>